<commit_message>
fix: bonus incoherence and logic problem
</commit_message>
<xml_diff>
--- a/assets/Map.xlsx
+++ b/assets/Map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26421"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/95d2f11f17913644/Documents/Études/LP/S1/Algorithmique/230323 PathFinder/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{FB42E16B-2132-4008-846F-C9DA228450B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55DA4330-0EDE-4C10-B5D5-C7051BA69904}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{FB42E16B-2132-4008-846F-C9DA228450B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB45CEC5-1D89-40F7-BF34-C6C27FFF5143}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="7200" yWindow="2415" windowWidth="21600" windowHeight="11295" xr2:uid="{4A55D093-698B-4091-AFAF-3773DFDC6DF4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4A55D093-698B-4091-AFAF-3773DFDC6DF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -297,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -344,13 +344,19 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -368,10 +374,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -674,15 +676,15 @@
   <dimension ref="A1:AB21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y19" sqref="Y19"/>
+      <selection activeCell="AB14" sqref="AB14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="21" width="4.7109375" customWidth="1"/>
+    <col min="1" max="21" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1">
         <v>1</v>
@@ -745,7 +747,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -813,13 +815,13 @@
         <v>0</v>
       </c>
       <c r="X2" s="17"/>
-      <c r="Z2" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA2" s="18"/>
-      <c r="AB2" s="17"/>
+      <c r="Z2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="19"/>
+      <c r="AB2" s="20"/>
     </row>
-    <row r="3" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -899,7 +901,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -979,7 +981,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1059,7 +1061,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1139,7 +1141,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1219,7 +1221,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1299,7 +1301,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1379,7 +1381,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1459,7 +1461,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1524,7 +1526,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1589,7 +1591,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1654,7 +1656,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1719,7 +1721,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1784,7 +1786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1849,7 +1851,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1914,7 +1916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1979,7 +1981,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2044,7 +2046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2109,7 +2111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
add Output.xlsx, Rapport.docx and implement a new rule
</commit_message>
<xml_diff>
--- a/assets/Map.xlsx
+++ b/assets/Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/95d2f11f17913644/Documents/Études/LP/S1/Algorithmique/230323 PathFinder/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{FB42E16B-2132-4008-846F-C9DA228450B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB45CEC5-1D89-40F7-BF34-C6C27FFF5143}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{FB42E16B-2132-4008-846F-C9DA228450B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{442AB1AF-1D7E-4654-B721-0B80F814BAF1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4A55D093-698B-4091-AFAF-3773DFDC6DF4}"/>
   </bookViews>
@@ -676,7 +676,7 @@
   <dimension ref="A1:AB21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB14" sqref="AB14"/>
+      <selection activeCell="Z20" sqref="Z20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>